<commit_message>
adding NL read capability
</commit_message>
<xml_diff>
--- a/extdata/toyFiles/FROC/bad/frocCr-01.xlsx
+++ b/extdata/toyFiles/FROC/bad/frocCr-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/PyJafroc/extdata/toyFiles/FROC/bad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E8C60F5-EFE9-C040-A191-5168877F130D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF10452-11FC-C94E-91B4-F80E755456A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11680" yWindow="4280" windowWidth="10000" windowHeight="9980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11680" yWindow="4280" windowWidth="10000" windowHeight="9980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LL" sheetId="3" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>ModalityID</t>
   </si>
   <si>
-    <t>FP_Rating</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>TP_Rating</t>
+  </si>
+  <si>
+    <t>NLRating</t>
   </si>
 </sst>
 </file>
@@ -585,15 +585,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>70</v>
@@ -607,10 +607,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>70</v>
@@ -624,10 +624,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>71</v>
@@ -641,10 +641,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>72</v>
@@ -658,10 +658,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>73</v>
@@ -675,10 +675,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>73</v>
@@ -692,10 +692,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>74</v>
@@ -709,10 +709,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>70</v>
@@ -726,10 +726,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>71</v>
@@ -743,10 +743,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>72</v>
@@ -760,10 +760,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1">
         <v>72</v>
@@ -777,10 +777,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1">
         <v>72</v>
@@ -794,10 +794,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1">
         <v>73</v>
@@ -811,10 +811,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1">
         <v>74</v>
@@ -828,10 +828,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1">
         <v>70</v>
@@ -845,10 +845,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1">
         <v>71</v>
@@ -862,10 +862,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1">
         <v>72</v>
@@ -879,10 +879,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1">
         <v>73</v>
@@ -896,10 +896,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1">
         <v>74</v>
@@ -913,10 +913,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1">
         <v>70</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1">
         <v>71</v>
@@ -947,10 +947,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1">
         <v>72</v>
@@ -964,10 +964,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1">
         <v>73</v>
@@ -981,10 +981,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="1">
         <v>74</v>
@@ -998,10 +998,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" s="1">
         <v>70</v>
@@ -1015,10 +1015,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1">
         <v>71</v>
@@ -1032,10 +1032,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1">
         <v>72</v>
@@ -1049,10 +1049,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1">
         <v>73</v>
@@ -1066,10 +1066,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" s="1">
         <v>74</v>
@@ -1083,10 +1083,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" s="1">
         <v>70</v>
@@ -1100,10 +1100,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" s="1">
         <v>71</v>
@@ -1133,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1156,15 +1156,15 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -1175,10 +1175,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -1189,10 +1189,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -1203,10 +1203,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -1217,10 +1217,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -1231,10 +1231,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -1245,10 +1245,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1259,10 +1259,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -1273,10 +1273,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -1287,10 +1287,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -1301,10 +1301,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
@@ -1315,10 +1315,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -1329,10 +1329,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -1343,10 +1343,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1">
         <v>74</v>
@@ -1357,10 +1357,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1">
         <v>73</v>
@@ -1371,10 +1371,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1">
         <v>3</v>
@@ -1385,10 +1385,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
@@ -1399,10 +1399,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
@@ -1413,10 +1413,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
@@ -1427,10 +1427,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1">
         <v>71</v>
@@ -1441,10 +1441,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1">
         <v>71</v>
@@ -1455,10 +1455,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1">
         <v>72</v>
@@ -1485,7 +1485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD8"/>
     </sheetView>
   </sheetViews>
@@ -1580,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
strange result reading character formatted cells
why do I need to convert cells to numeric?
</commit_message>
<xml_diff>
--- a/extdata/toyFiles/FROC/bad/frocCr-01.xlsx
+++ b/extdata/toyFiles/FROC/bad/frocCr-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/PyJafroc/extdata/toyFiles/FROC/bad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF10452-11FC-C94E-91B4-F80E755456A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E218397E-8B27-314B-93CC-73C9301EFAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11680" yWindow="4280" windowWidth="10000" windowHeight="9980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,10 +61,10 @@
     <t>2</t>
   </si>
   <si>
-    <t>TP_Rating</t>
+    <t>NLRating</t>
   </si>
   <si>
-    <t>NLRating</t>
+    <t>LLRating</t>
   </si>
 </sst>
 </file>
@@ -560,7 +560,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -585,7 +585,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1156,7 +1156,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>